<commit_message>
Bad link error fixed
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -14,7 +14,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="25">
   <si>
     <t>Asign</t>
   </si>
@@ -49,13 +49,65 @@
   </si>
   <si>
     <t>Min price</t>
+  </si>
+  <si>
+    <t>https://www.walmart.com/ip/IRWIN-VISE-GRIP-2076709-Fast-Release-Locking-Plier-Set-6Pc/40751123</t>
+  </si>
+  <si>
+    <t>https://www.walmart.com/ip/CHAMBERLAIN-CWA2000-Wireless-Motion-Alert-System/14554538</t>
+  </si>
+  <si>
+    <t>https://www.walmart.com/ip/Air-Purifier-Hepa-Carbon-Ionic-Ozone-Generator-Cleaner-UV-C-with-Remote/179032464</t>
+  </si>
+  <si>
+    <t>https://www.walmart.com/ip/4PC-Self-Adjusting-Quick-Release-Pipe-Wrench-Drop-Forge-Plumbing/193316668</t>
+  </si>
+  <si>
+    <t>https://www.walmart.com/ip/Torque-Multiplier-Wrench-Lug-Nut-Remover-with-4-cr-v-sockets/102917115</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Availability</t>
+  </si>
+  <si>
+    <t>Purchased</t>
+  </si>
+  <si>
+    <t>Undefined</t>
+  </si>
+  <si>
+    <t>Something wrong with this listing. Check it by yourself!</t>
+  </si>
+  <si>
+    <t>Air Purifier Hepa Carbon Ionic Ozone Generator Cleaner UV-C, with Remote</t>
+  </si>
+  <si>
+    <t>97,93</t>
+  </si>
+  <si>
+    <t>Availible</t>
+  </si>
+  <si>
+    <t>4PC Self-Adjusting Quick Release Pipe Wrench Drop Forge Plumbing</t>
+  </si>
+  <si>
+    <t>49,93</t>
+  </si>
+  <si>
+    <t>Torque Multiplier Wrench Lug Nut Remover, with 4 cr-v sockets</t>
+  </si>
+  <si>
+    <t>53,93</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +122,14 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,16 +164,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -392,15 +459,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="17" customWidth="1" collapsed="1"/>
+    <col min="1" max="8" customWidth="true" width="17.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -428,9 +495,148 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>